<commit_message>
Version mit allen AuswahlMenus und Markern
</commit_message>
<xml_diff>
--- a/hofverkauf/Hofverkauf.xlsx
+++ b/hofverkauf/Hofverkauf.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4629" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4630" uniqueCount="381">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1491,8 +1491,8 @@
   </sheetPr>
   <dimension ref="A2:CD65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G65" activeCellId="0" sqref="G65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ66" activeCellId="0" sqref="AJ66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16119,6 +16119,9 @@
       <c r="L65" s="19"/>
       <c r="M65" s="19"/>
       <c r="N65" s="19"/>
+      <c r="AJ65" s="15" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>